<commit_message>
docs: use case description fix - use case description fix
</commit_message>
<xml_diff>
--- a/문재영/requirement_list_mun_jaeyoung.xlsx
+++ b/문재영/requirement_list_mun_jaeyoung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\answodud\Desktop\se2\SE_Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACB903A-B8D7-4080-83B0-705922A06F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F1EACD-5B11-4924-AE36-25D5A2E3D2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{874C0683-1278-4AE4-B97F-6F37D411C365}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{874C0683-1278-4AE4-B97F-6F37D411C365}"/>
   </bookViews>
   <sheets>
     <sheet name="main usecase requirement list" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>예약 대기 취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>System Response</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대여 기록 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기록 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원은 현재 대여 중인 자전거 목록을 조회 가능하다. 각 목록에는 대여소 이름, 대여소 위치, 자전거 ID, 자전거 제품명, 자전거 유형 정보가 있다. 이 중 원하는 자전거를 반납할 수 있다. 반납 시 사용 시간에 따라 요금이 자동 결제된다. 반납 완료된 자전거의 대기 1순위 회원에게 예약 이메일을 전송한다. 반납 후 원하는 경우 근처 식당을 추천 받아서 예약 가능한 외부 서비스에 연결된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원은 예약 대기를 신청한 자전거 목록을 조회 가능하다. 목록에는 대여소 이름, 대여소 위치, 자전거 ID, 자전거 제품명, 자전거 유형 정보가 있다. 특정 자전거를 선택하여 예약 대기를 취소할 수 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -115,99 +103,143 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. 현재 회원이 예약 대기 중인 자전거 리스트와 각 자전거의 &lt;예약 대기 취소&gt; 버튼을 출력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Actor Action(회원)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3. "해당 대여 기록을 정말 삭제하시겠습니까?" 라는 팝업을 띄운다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. "대여 기록이 삭제 되었습니다" 라는 팝업을 띄운다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6. &lt;대여소 별로 정렬&gt; 버튼을 클릭한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. &lt;확인&gt; 버튼을 클릭한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">3. "해당 예약 대기를 정말 취소하시겠습니까?" 라는 문구의 팝업을 띄운다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 예약 대기를 취소하고 싶은 자전거의 &lt;예약 대기 취소&gt; 버튼을 클릭한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. "예약 대기가 취소되었습니다." 라는 문구의 팝업을 띄운다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 삭제하고 싶은 대여 기록의 &lt;삭제&gt; 버튼을 클릭한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 과거 대여 기록 리스트와 대여 기록의 &lt;삭제&gt; 버튼을 날짜 별로 출력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. 과거 대여 기록 리스트와 대여 기록의 &lt;삭제&gt; 버튼을 대여소 별로 출력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 반납하고 싶은 자전거의 &lt;반납&gt; 버튼을 클릭한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. "반납하시겠습니까?" 라는 문구의 팝업을 띄운다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. 자동 결제 시스템에 사용 시간과 함께 결제 요청을 보낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">9. "반납이 완료되었습니다." 라는 문구와 &lt;반납 대여소 근처 식당 추천받기&gt; 버튼이 함께 있는 팝업을 띄운다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10. &lt;반납 대여소 근처 식당 추천받기&gt; 버튼을 클릭한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11. 식당 예약 시스템에 요청을 보낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8. 대기 1순위 회원에게 이메일 전송 후 완료 응답을 보낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">6. 결제 완료 후 응답을 보낸다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 현재 대여 중인 자전거 리스트와 각 자전거의 &lt;반납&gt; 버튼을 자전거 ID 순으로 출력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. 반납이 완료된 자전거에 예약 대기가 있을 경우 대기 1순위 회원 정보와 함께 이메일 발송 시스템에 요청을 보낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12. 식당 예약 시스템 페이지를 띄운다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 회원이 마지막으로 반납한 자전거의 대여 시간과 요금을 출력한다.</t>
+    <t>1. &lt;대여 자전거 조회&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 현재 대여 중인 자전거 리스트와 각 자전거의 &lt;반납&gt; 버튼을 자전거 ID 순으로 출력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 반납하고 싶은 자전거의 &lt;반납&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. "반납하시겠습니까?" 라는 문구의 팝업을 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. &lt;확인&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 자동 결제 시스템에 사용 시간과 함께 결제 요청을 보낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">7. 결제 완료 후 응답을 보낸다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. 반납이 완료된 자전거에 예약 대기가 있을 경우 대기 1순위 회원 정보와 함께 이메일 발송 시스템에 요청을 보낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. 대기 1순위 회원에게 이메일 전송 후 완료 응답을 보낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">12. "반납이 완료되었습니다." 라는 문구와 &lt;반납 대여소 근처 식당 추천받기&gt; 버튼이 함께 있는 팝업을 띄운다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13. &lt;반납 대여소 근처 식당 추천받기&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14. 식당 예약 시스템에 요청을 보낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15. 식당 예약 시스템 페이지를 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대여 자전거 조회(usecase #1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약 대기 취소(usecase #2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. &lt;예약 대기 취소하기&gt; 버튼을 누른다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 현재 회원이 예약 대기 중인 자전거 리스트와 각 자전거의 &lt;예약 대기 취소&gt; 버튼을 출력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 예약 대기를 취소하고 싶은 자전거의 &lt;예약 대기 취소&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4. "해당 예약 대기를 정말 취소하시겠습니까?" 라는 문구의 팝업을 띄운다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. "예약 대기가 취소되었습니다." 라는 문구의 팝업을 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. &lt;요금 조회&gt; 버튼을 누른다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 회원이 마지막으로 반납한 자전거의 대여 시간과 요금을 출력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요금 조회(usecase #3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대여 기록 조회(usecase #4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. &lt;대여 기록 조회&gt; 버튼을 누른다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 과거 대여 기록 리스트와 대여 기록의 &lt;삭제&gt; 버튼을 날짜 별로 출력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 삭제하고 싶은 대여 기록의 &lt;삭제&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. "해당 대여 기록을 정말 삭제하시겠습니까?" 라는 팝업을 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. "대여 기록이 삭제 되었습니다" 라는 팝업을 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. &lt;대여소 별로 정렬&gt; 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. 과거 대여 기록 리스트와 대여 기록의 &lt;삭제&gt; 버튼을 대여소 별로 출력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. [요금 조회](usecase #3) 화면을 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. [요금 조회](usecase #3) 화면을 닫는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원은 현재 대여 중인 자전거 목록을 조회 가능하다. 각 목록에는 대여소 이름, 대여소 위치, 자전거 ID, 자전거 제품명, 자전거 유형 정보가 있다. 이 중 원하는 자전거를 반납할 수 있다. 반납 시 사용 시간에 따라 요금이 자동 결제된다. 결제 후 반납 자전거의 요금 조회 화면이 뜬다. 반납 완료된 자전거의 대기 1순위 회원에게 예약 이메일을 전송한다. 반납 후 원하는 경우 근처 식당을 추천 받아서 예약 가능한 외부 서비스에 연결된다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -350,7 +382,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -394,6 +426,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -732,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BE2212-1D95-40D6-8E41-4E4FEC407314}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -753,15 +803,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="102" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="119" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="95.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -769,10 +819,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.45">
@@ -780,7 +830,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -791,10 +841,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -830,10 +880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707464CE-9566-4202-8AA3-4A9A17F1FF36}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="78" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -848,7 +898,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -857,227 +907,266 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.45">
+      <c r="A4" s="10"/>
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A6" s="10"/>
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A8" s="10"/>
+      <c r="E8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.45">
+      <c r="A10" s="10"/>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A11" s="10"/>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A12" s="10"/>
+      <c r="E12" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.45">
+      <c r="A14" s="10"/>
+      <c r="E14" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.45">
+      <c r="A15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A16" s="10"/>
+      <c r="E16" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A17" s="11"/>
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.45">
-      <c r="A3" s="10"/>
-      <c r="E3" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.45">
-      <c r="A5" s="10"/>
-      <c r="E5" s="6" t="s">
+      <c r="B22" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A23" s="15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.45">
-      <c r="A7" s="10"/>
-      <c r="E7" s="7" t="s">
+      <c r="B23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.45">
+      <c r="A24" s="10"/>
+      <c r="B24" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="10"/>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.45">
-      <c r="A9" s="10"/>
-      <c r="E9" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.45">
-      <c r="A10" s="10"/>
-      <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.45">
-      <c r="A11" s="10"/>
-      <c r="E11" s="6" t="s">
+    <row r="25" spans="1:5" ht="68" x14ac:dyDescent="0.45">
+      <c r="A25" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.45">
+      <c r="A26" s="10"/>
+      <c r="B26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.45">
-      <c r="A13" s="10"/>
-      <c r="E13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
-      <c r="B14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="51" x14ac:dyDescent="0.45">
-      <c r="A20" s="10"/>
-      <c r="B20" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="68" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" ht="51" x14ac:dyDescent="0.45">
-      <c r="A22" s="10"/>
-      <c r="B22" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
-      <c r="B24" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="13"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.45">
       <c r="A28" s="11"/>
       <c r="B28" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="13"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.45">
+      <c r="A32" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="20"/>
+    </row>
+    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="A33" s="11"/>
+      <c r="B33" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="13"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="A39" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="17"/>
+    </row>
+    <row r="40" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+      <c r="A40" s="10"/>
+      <c r="B40" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="13"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.45">
-      <c r="A34" s="10"/>
-      <c r="B34" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="51" x14ac:dyDescent="0.45">
-      <c r="A35" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2" ht="34" x14ac:dyDescent="0.45">
-      <c r="A36" s="10"/>
-      <c r="B36" s="6" t="s">
+    <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+      <c r="A41" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="A42" s="10"/>
+      <c r="B42" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="A43" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="34" x14ac:dyDescent="0.45">
-      <c r="A37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" ht="34" x14ac:dyDescent="0.45">
-      <c r="A38" s="10"/>
-      <c r="B38" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="34" x14ac:dyDescent="0.45">
-      <c r="A39" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="1:2" ht="51" x14ac:dyDescent="0.45">
-      <c r="A40" s="11"/>
-      <c r="B40" s="9" t="s">
-        <v>30</v>
+      <c r="B43" s="6"/>
+    </row>
+    <row r="44" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="A44" s="10"/>
+      <c r="B44" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="A45" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+      <c r="A46" s="11"/>
+      <c r="B46" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>